<commit_message>
dernieres modif de Pierre
lecture des roles dans un document texte,  ajout de l'icone de dragon dans toutes les frames, et d'autres petites modifs mais je m'en souviens plus
</commit_message>
<xml_diff>
--- a/classes/Classeur1.xlsx
+++ b/classes/Classeur1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierre\Desktop\Projet-informatique-ClassCraft-mariogamer\classes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierre\Desktop\Projet-informatique-ClassCraft\classes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA901C2-A345-40C3-B580-4C2115226E94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34C205A-48F7-4494-9346-D7D69EABA8E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -455,7 +455,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Project has been yoten
</commit_message>
<xml_diff>
--- a/classes/Classeur1.xlsx
+++ b/classes/Classeur1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="37">
   <si>
     <t>Numéros d'admission</t>
   </si>
@@ -47,7 +47,7 @@
     <t>4444</t>
   </si>
   <si>
-    <t xml:space="preserve">bobette </t>
+    <t xml:space="preserve">zbobette </t>
   </si>
   <si>
     <t>rocher</t>
@@ -178,12 +178,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -286,10 +289,10 @@
       </c>
       <c r="E4"/>
       <c r="F4" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G4" t="n">
-        <v>5.0</v>
+        <v>31.0</v>
       </c>
       <c r="H4" t="n">
         <v>3.0</v>
@@ -301,10 +304,10 @@
         <v>6</v>
       </c>
       <c r="K4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="L4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="M4" t="s">
         <v>6</v>
@@ -1213,7 +1216,7 @@
         <v>1.0</v>
       </c>
       <c r="G26" t="n">
-        <v>5.0</v>
+        <v>20.0</v>
       </c>
       <c r="H26" t="n">
         <v>2.0</v>

</xml_diff>